<commit_message>
Readme update and comments
</commit_message>
<xml_diff>
--- a/RunScenarioFromAnotherTest/MasterTest.rvl.xlsx
+++ b/RunScenarioFromAnotherTest/MasterTest.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t>Flow</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>Login</t>
   </si>
 </sst>
 </file>
@@ -483,7 +486,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>10</v>

</xml_diff>